<commit_message>
Add static blank plot, GUI in main thread instead of separate thread
</commit_message>
<xml_diff>
--- a/config/config.xlsx
+++ b/config/config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PRussell\PycharmProjects\Lesson1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PRussell\PycharmProjects\SHED_2020\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5408656E-0B3C-4DD1-9B12-76C56347873D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F69D8A04-EE15-4ECB-8800-E48CE53D0F0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="0" windowWidth="10656" windowHeight="9000" xr2:uid="{82A4BAAA-6ED8-4E76-AA6A-33CFEDDEFD2A}"/>
+    <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{82A4BAAA-6ED8-4E76-AA6A-33CFEDDEFD2A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -583,8 +583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7068524D-5CCD-4349-A0BD-476FA9D60713}">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -611,7 +611,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>100</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -870,7 +870,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C548B4C-BA48-40B5-B431-A1AA20E76153}">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Flow/Alarm/Exhaust/SHEDstatus complete on Class_try -Working main SHED controller
</commit_message>
<xml_diff>
--- a/config/config.xlsx
+++ b/config/config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PRussell\PycharmProjects\SHED_2020\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F69D8A04-EE15-4ECB-8800-E48CE53D0F0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27CFA7A1-CE83-4E1A-9612-08B6C54B2804}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{82A4BAAA-6ED8-4E76-AA6A-33CFEDDEFD2A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="75">
   <si>
     <t>SHED Auxiliary systems config file</t>
   </si>
@@ -220,6 +220,45 @@
   </si>
   <si>
     <t>// Valve voltage which corresponding pump turns off to protect against deadheading</t>
+  </si>
+  <si>
+    <t>Flow Temperature Range</t>
+  </si>
+  <si>
+    <t>SHED3 Hot</t>
+  </si>
+  <si>
+    <t>SHED3 Cold</t>
+  </si>
+  <si>
+    <t>SHED2 Hot</t>
+  </si>
+  <si>
+    <t>SHED2 Cold</t>
+  </si>
+  <si>
+    <t>Main Hot</t>
+  </si>
+  <si>
+    <t>Main Cold</t>
+  </si>
+  <si>
+    <t>SHED1 Cold</t>
+  </si>
+  <si>
+    <t>SHED1 Hot</t>
+  </si>
+  <si>
+    <t>Lower bound</t>
+  </si>
+  <si>
+    <t>Higher Bound</t>
+  </si>
+  <si>
+    <t>Flow Rate Range</t>
+  </si>
+  <si>
+    <t>Lower Bound</t>
   </si>
 </sst>
 </file>
@@ -240,15 +279,27 @@
       <name val="JetBrains Mono"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -256,17 +307,165 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -581,10 +780,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7068524D-5CCD-4349-A0BD-476FA9D60713}">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -611,7 +810,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>1000</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -858,6 +1057,205 @@
       </c>
       <c r="C23" t="s">
         <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="15" thickBot="1"/>
+    <row r="26" spans="1:9">
+      <c r="A26" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B27" s="4">
+        <v>50</v>
+      </c>
+      <c r="C27" s="9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B28" s="4">
+        <v>0</v>
+      </c>
+      <c r="C28" s="9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B29" s="4">
+        <v>50</v>
+      </c>
+      <c r="C29" s="9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" s="4">
+        <v>0</v>
+      </c>
+      <c r="C30" s="9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B31" s="4">
+        <v>50</v>
+      </c>
+      <c r="C31" s="9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B32" s="4">
+        <v>0</v>
+      </c>
+      <c r="C32" s="9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B33" s="4">
+        <v>0</v>
+      </c>
+      <c r="C33" s="9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="15" thickBot="1">
+      <c r="A34" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B34" s="11">
+        <v>50</v>
+      </c>
+      <c r="C34" s="12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B37" s="15">
+        <v>0.01</v>
+      </c>
+      <c r="C37" s="15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B38" s="15">
+        <v>0.01</v>
+      </c>
+      <c r="C38" s="15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="B39" s="15">
+        <v>0.01</v>
+      </c>
+      <c r="C39" s="15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="B40" s="15">
+        <v>0.01</v>
+      </c>
+      <c r="C40" s="15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="B41" s="15">
+        <v>0.01</v>
+      </c>
+      <c r="C41" s="15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="B42" s="15">
+        <v>0.01</v>
+      </c>
+      <c r="C42" s="15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="B43" s="15">
+        <v>0.01</v>
+      </c>
+      <c r="C43" s="15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="15" thickBot="1">
+      <c r="A44" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="B44" s="15">
+        <v>0.01</v>
+      </c>
+      <c r="C44" s="15">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>